<commit_message>
Doplneny obrazky k jednotlivym uloham.
</commit_message>
<xml_diff>
--- a/cvikaVES/el_obvody/vypocet.xlsx
+++ b/cvikaVES/el_obvody/vypocet.xlsx
@@ -412,7 +412,7 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,23 +575,23 @@
         <v>12</v>
       </c>
       <c r="M4">
-        <v>1.1599999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="N4">
         <f>M4/L4</f>
-        <v>9.6666666666666665E-2</v>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="O4">
         <f>N4/(1-N4)</f>
-        <v>0.1070110701107011</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="P4">
         <f>(I4+I4*O4)/O4</f>
-        <v>34834.623504574243</v>
+        <v>33673.469387755104</v>
       </c>
       <c r="Q4">
         <f>O4*P4</f>
-        <v>3727.6903381278707</v>
+        <v>3741.4965986394559</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -638,23 +638,23 @@
         <v>12</v>
       </c>
       <c r="M5">
-        <v>1.1599999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="N5">
         <f t="shared" ref="N5:N8" si="5">M5/L5</f>
-        <v>9.6666666666666665E-2</v>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="O5">
         <f t="shared" ref="O5:O8" si="6">N5/(1-N5)</f>
-        <v>0.1070110701107011</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="P5">
         <f>(I5+I5*O5)/O5</f>
-        <v>22312.373225152129</v>
+        <v>21568.627450980392</v>
       </c>
       <c r="Q5">
         <f t="shared" ref="Q5:Q8" si="7">O5*P5</f>
-        <v>2387.6709355328844</v>
+        <v>2396.5141612200432</v>
       </c>
       <c r="R5">
         <v>22000</v>
@@ -719,23 +719,23 @@
         <v>12</v>
       </c>
       <c r="M6">
-        <v>1.1599999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="N6">
         <f t="shared" si="5"/>
-        <v>9.6666666666666665E-2</v>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="O6">
         <f t="shared" si="6"/>
-        <v>0.1070110701107011</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="P6">
         <f>(I6+I6*O6)/O6</f>
-        <v>13952.832847881238</v>
+        <v>13487.738419618528</v>
       </c>
       <c r="Q6">
         <f t="shared" si="7"/>
-        <v>1493.1075741275124</v>
+        <v>1498.6376021798364</v>
       </c>
       <c r="R6">
         <v>15000</v>
@@ -800,23 +800,23 @@
         <v>12</v>
       </c>
       <c r="M7">
-        <v>1.1599999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="N7">
         <f t="shared" si="5"/>
-        <v>9.6666666666666665E-2</v>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="O7">
         <f t="shared" si="6"/>
-        <v>0.1070110701107011</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="P7">
         <f>(I7+I7*O7)/O7</f>
-        <v>7976.1521108604575</v>
+        <v>7710.2803738317762</v>
       </c>
       <c r="Q7">
         <f t="shared" si="7"/>
-        <v>853.53657274890497</v>
+        <v>856.69781931464172</v>
       </c>
       <c r="R7">
         <v>8200</v>
@@ -881,35 +881,35 @@
         <v>12</v>
       </c>
       <c r="M8">
-        <v>1.1599999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="N8">
         <f t="shared" si="5"/>
-        <v>9.6666666666666665E-2</v>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="O8">
         <f t="shared" si="6"/>
-        <v>0.1070110701107011</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="P8">
         <f>(I8+I8*O8)/O8</f>
-        <v>3490.5859953458857</v>
+        <v>3374.2331288343557</v>
       </c>
       <c r="Q8">
         <f t="shared" si="7"/>
-        <v>373.53134267538996</v>
+        <v>374.91479209270619</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="Q10">
         <f>Q5-2200</f>
-        <v>187.67093553288441</v>
+        <v>196.51416122004321</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="Q11">
         <f>Q5-2700</f>
-        <v>-312.32906446711559</v>
+        <v>-303.48583877995679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
První tři úlohy jsou plně popsány, pájení se popisovat víc nebude. Je třeba dodělat polovodiče a fotovoltaické panely.
</commit_message>
<xml_diff>
--- a/cvikaVES/el_obvody/vypocet.xlsx
+++ b/cvikaVES/el_obvody/vypocet.xlsx
@@ -412,7 +412,7 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,26 +572,26 @@
         <v>1.3499999999999998E-7</v>
       </c>
       <c r="L4">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M4">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="N4">
         <f>M4/L4</f>
-        <v>9.9999999999999992E-2</v>
+        <v>8.666666666666667E-2</v>
       </c>
       <c r="O4">
         <f>N4/(1-N4)</f>
-        <v>0.1111111111111111</v>
+        <v>9.4890510948905119E-2</v>
       </c>
       <c r="P4">
         <f>(I4+I4*O4)/O4</f>
-        <v>33673.469387755104</v>
+        <v>38854.003139717424</v>
       </c>
       <c r="Q4">
         <f>O4*P4</f>
-        <v>3741.4965986394559</v>
+        <v>3686.87621033815</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -635,26 +635,26 @@
         <v>1.7249999999999999E-7</v>
       </c>
       <c r="L5">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M5">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="N5">
         <f t="shared" ref="N5:N8" si="5">M5/L5</f>
-        <v>9.9999999999999992E-2</v>
+        <v>8.666666666666667E-2</v>
       </c>
       <c r="O5">
         <f t="shared" ref="O5:O8" si="6">N5/(1-N5)</f>
-        <v>0.1111111111111111</v>
+        <v>9.4890510948905119E-2</v>
       </c>
       <c r="P5">
         <f>(I5+I5*O5)/O5</f>
-        <v>21568.627450980392</v>
+        <v>24886.877828054294</v>
       </c>
       <c r="Q5">
         <f t="shared" ref="Q5:Q8" si="7">O5*P5</f>
-        <v>2396.5141612200432</v>
+        <v>2361.5285530270498</v>
       </c>
       <c r="R5">
         <v>22000</v>
@@ -716,26 +716,26 @@
         <v>2.3499999999999995E-7</v>
       </c>
       <c r="L6">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M6">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="N6">
         <f t="shared" si="5"/>
-        <v>9.9999999999999992E-2</v>
+        <v>8.666666666666667E-2</v>
       </c>
       <c r="O6">
         <f t="shared" si="6"/>
-        <v>0.1111111111111111</v>
+        <v>9.4890510948905119E-2</v>
       </c>
       <c r="P6">
         <f>(I6+I6*O6)/O6</f>
-        <v>13487.738419618528</v>
+        <v>15562.77509955984</v>
       </c>
       <c r="Q6">
         <f t="shared" si="7"/>
-        <v>1498.6376021798364</v>
+        <v>1476.759680980131</v>
       </c>
       <c r="R6">
         <v>15000</v>
@@ -744,15 +744,15 @@
         <v>1500</v>
       </c>
       <c r="T6">
-        <f t="shared" ref="T6:T7" si="9">S6*R6/(R6+S6)</f>
+        <f>S6*R6/(R6+S6)</f>
         <v>1363.6363636363637</v>
       </c>
       <c r="U6">
-        <f t="shared" ref="U6:U7" si="10">T6*B6/(T6+B6)</f>
+        <f>T6*B6/(T6+B6)</f>
         <v>964.9122807017543</v>
       </c>
       <c r="V6" s="1">
-        <f t="shared" ref="V6:V7" si="11">C6*A6/U6</f>
+        <f>C6*A6/U6</f>
         <v>2.3318181818181817E-7</v>
       </c>
     </row>
@@ -797,26 +797,26 @@
         <v>3.5999999999999994E-7</v>
       </c>
       <c r="L7">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M7">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="N7">
         <f t="shared" si="5"/>
-        <v>9.9999999999999992E-2</v>
+        <v>8.666666666666667E-2</v>
       </c>
       <c r="O7">
         <f t="shared" si="6"/>
-        <v>0.1111111111111111</v>
+        <v>9.4890510948905119E-2</v>
       </c>
       <c r="P7">
         <f>(I7+I7*O7)/O7</f>
-        <v>7710.2803738317762</v>
+        <v>8896.4773544212785</v>
       </c>
       <c r="Q7">
         <f t="shared" si="7"/>
-        <v>856.69781931464172</v>
+        <v>844.19128180639882</v>
       </c>
       <c r="R7">
         <v>8200</v>
@@ -825,15 +825,15 @@
         <v>820</v>
       </c>
       <c r="T7">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="T6:T7" si="9">S7*R7/(R7+S7)</f>
         <v>745.4545454545455</v>
       </c>
       <c r="U7">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="U6:U7" si="10">T7*B7/(T7+B7)</f>
         <v>608.08988764044943</v>
       </c>
       <c r="V7" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="V6:V7" si="11">C7*A7/U7</f>
         <v>3.7001108647450107E-7</v>
       </c>
     </row>
@@ -878,38 +878,52 @@
         <v>7.3499999999999995E-7</v>
       </c>
       <c r="L8">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M8">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="N8">
         <f t="shared" si="5"/>
-        <v>9.9999999999999992E-2</v>
+        <v>8.666666666666667E-2</v>
       </c>
       <c r="O8">
         <f t="shared" si="6"/>
-        <v>0.1111111111111111</v>
+        <v>9.4890510948905119E-2</v>
       </c>
       <c r="P8">
         <f>(I8+I8*O8)/O8</f>
-        <v>3374.2331288343557</v>
+        <v>3893.3459178857947</v>
       </c>
       <c r="Q8">
         <f t="shared" si="7"/>
-        <v>374.91479209270619</v>
+        <v>369.44158344901706</v>
+      </c>
+      <c r="T8">
+        <f>P5*Q5/(P5+Q5)</f>
+        <v>2156.8627450980389</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T9">
+        <f>P6*Q6/(P6+Q6)</f>
+        <v>1348.7738419618529</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="Q10">
         <f>Q5-2200</f>
-        <v>196.51416122004321</v>
+        <v>161.52855302704984</v>
+      </c>
+      <c r="T10">
+        <f>P7*Q7/(P7+Q7)</f>
+        <v>771.02803738317755</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="Q11">
         <f>Q5-2700</f>
-        <v>-303.48583877995679</v>
+        <v>-338.47144697295016</v>
       </c>
     </row>
   </sheetData>

</xml_diff>